<commit_message>
wrote script to extract year names and write them to excel
</commit_message>
<xml_diff>
--- a/tabulatedData.xlsx
+++ b/tabulatedData.xlsx
@@ -3,10 +3,11 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="testSheetNames" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="testSheetYears" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -426,7 +427,7 @@
   </sheetPr>
   <dimension ref="A1:R10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
@@ -937,4 +938,255 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:R10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>TABID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>NOYEARS</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>P509633.conll</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mu {d}nin-urta u3 ma-na-ba-al-te-el in-pa3 igi ia-ah-zi-be2-el3 dumu isz-me-{d}suen igi szu-la-ra-ak igi na-nu-szu-um dumu za-x-la-nu igi ku-nu-um dumu nu-ur2-ia </t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mu e2 {d}nin-urta ma-na-ba-al-te-el mu-na-du3 dumu isz-me-{d}suen igi szu-la-ra-ak dumu x-x-x-x igi ku-nu-um dumu nu-ur2-ia ... x ... </t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>P509634.conll</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>P509636.conll</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mu {gesz}gu-za za3-bi-us2 3(disz)-a-bi {d}en-lil2 {d}nin-urta {d}nin-nibru{ki} ma-na-ba-al-te-el {disz}{d}suen-a-hu-szu u3 sza-at-{d}gibil6 ha-la e2 ad-da-ni nig2 na-me ugu za-za-kum li-bi2-in-tuku igi a-mur-i-lu-su2 igi {d}suen-en-nam szitim igi bur-ia dumu sa-li igi {d}nanna-zi-sza3-gal2 iti gan-gan-e3 </t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mu {gesz}gu-za za3-bi-us2 3(disz)-a-bi {d}en-lil2 {d}nin-urta {d}nin-nibru{ki} ma-na-dim2 {d}suen-a-bu-szu dumu za-pa-ti </t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>P509663.conll</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mu ma-ma-ba-al-te-el 6(disz) gin2 ku3-babbar sa10 2(asz) gur sze szu ti-a a-na-gum </t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mu mu-na-ba-al-te-el 1(u) 3(disz) 1/2(disz) gin2 1(disz)-kam 1(u) 3(disz) 1/3(disz) gin2 2(disz)-kam 1/3(disz) ma-na 8(disz) igi-6(disz)-gal2 szu-la2 </t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mu ma-na-ba-al-te-el </t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>P509664.conll</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>P509668.conll</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>P509669.conll</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mu ... 4(disz) gu4-ab2 6(disz) ab2 mah2 2(u) 7(disz) gu4 amar-ga 1(disz) amar nig2 e2 nam-ra-tum nig2-szu la-lum giri3 x-x-x-x i3-gen-ne-en iti sze-sag11-ku5 u4 4(disz)-kam </t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mu GISZ ... la-lu-um dumu sa-al-lum </t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>P509670.conll</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mu ... 4(disz) ab2 mah2 6(disz) gu4-ab2 2(u) 2(disz) ab2 amar-ga 6(disz) gu4 amar-ga 3(u) 8(disz) gu4 ab2 amar-hi-a nig2-szu {d}utu-sipa </t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>P509671.conll</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>16</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mu 1(disz) 2(disz) gu4 </t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mu 2(disz) 1(disz) gu4 </t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mu 1(disz) 1(disz) gu4 amar-ga 1(disz) ab2 amar-ga 1(u) 1(disz) gu4 ab2 amar dingir-na-sir 2(disz) ab2 mah2 2(disz) ab2 </t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mu 1(disz) 1(disz) ab2 amar-ga 1(disz) gu4 amar-ga 6(disz) er3-ra-ha-bi-it 4(disz) ab2 mah2 2(disz) ab2 amar-ga 1(disz) gu4 amar-ga n ab2 amar-ga n ab2 </t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mu n n gu4 </t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mu 2(disz) 1(disz) gu4 </t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mu 1(disz) 1(disz) gu4 amar-ga 1(disz) ab2 amar-ga 8(disz) a-hu-um-ma 1(disz) ab2 mah2 1(disz) gu4 </t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mu 3(disz) 1(disz) gu4 </t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mu 1(disz) 1(disz) ab2 amar-ga 4(disz) {d}suen-na-si-ir 2(disz) ab2 mah2 2(disz) ab2 </t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mu 2(disz) 1(disz) gu4 </t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mu n 5(disz) sza3 2(u) a-ra2 1(disz)-kam 5(disz) ab2 mah2 2(disz) ab2 </t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mu 2(disz) 2(disz) ab2 </t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mu 1(disz) 2(disz) gu4 </t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mu 1(disz) 3(disz) gu4 </t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mu 2(disz) 3(disz) gu4 </t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mu 3(disz) 1(u) 7(disz) x ... nig2-szu {d}suen-x-x </t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
year matcher with expected behavior
</commit_message>
<xml_diff>
--- a/tabulatedData.xlsx
+++ b/tabulatedData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="1" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2080" yWindow="2080" windowWidth="14400" windowHeight="7360" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="tablets&amp;Names" sheetId="1" state="visible" r:id="rId1"/>
@@ -426,10 +426,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R10"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
@@ -449,97 +449,67 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>P509633.conll</t>
+          <t>P122472.conll</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{disz}{d}suen-sze-mi</t>
+          <t>ur-sukkal</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>um-mi-he-pa2-at</t>
+          <t>BI</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>in-szi-sa10</t>
+          <t>da-da</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>in-pa3</t>
+          <t>ur-{d}dumu-zi-da</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>ia-ah-zi-be2-el3</t>
+          <t>...</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>isz-me-{d}suen</t>
+          <t>...</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>szu-la-ra-ak</t>
+          <t>...</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>na-nu-szu-um</t>
+          <t>...</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>za-x-la-nu</t>
+          <t>lu2-ma2-gur8-re</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>ku-nu-um</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>nu-ur2-ia</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>isz-me-{d}suen</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>szu-la-ra-ak</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>x-x-x-x</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>ku-nu-um</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>nu-ur2-ia</t>
+          <t>e2-di</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>P509634.conll</t>
+          <t>P122473.conll</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -547,279 +517,139 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>i-x-x-x-x</t>
+          <t>la2-ia3</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>me-x-x-x</t>
+          <t>ur-{d}szul-pa-e3</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>zi-x-x-x-x</t>
+          <t>ma2-gur8-mah</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>NI-x-x-x</t>
+          <t>ur-{d}szul-pa-e3</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>in-szi-sa10</t>
+          <t>a-tu</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>P509636.conll</t>
+          <t>P122474.conll</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>{disz}{d}suen-a-hu-szu</t>
+          <t>a-iri-mu</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>sza-at-{d}gibil6</t>
+          <t>{d}szul-gi-ba-ni</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>a-mur-i-lu-su2</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>bur-ia</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>sa-li</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>{d}nanna-zi-sza3-gal2</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>{disz}{d}suen-a-hu-szu</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>sza-at-{d}gibil6</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>a-mur-i-lu-su2</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>bur-ia</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>sa-li</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>{d}nanna-zi-sza3-gal2</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>{d}suen-a-bu-szu</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>za-pa-ti</t>
+          <t>a-ta2-kal2-szum</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>P509663.conll</t>
+          <t>P122475.conll</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>bu-sum</t>
+          <t>ha-bu3-da</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>ma-ma-ba-al-te-el</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>a-na-gum</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>szu-la2</t>
+          <t>ur-du6-ku3-ga</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>P509664.conll</t>
+          <t>P122476.conll</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>a-hi-i-ma</t>
+          <t>NE</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>a-hi-i-ma</t>
+          <t>szu-numun-ka</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>a-hi-i-ma</t>
+          <t>ur-{d}nusku-ra</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>an-na-ab-szum2-mu</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>P509668.conll</t>
+          <t>P122477.conll</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>8</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>bur-ru-um</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>{d}suen-gi-im-la-an-ni</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>{d}suen-i-din-nam</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>{d}suen-szar-rum</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>a-bi-ia</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>{d}suen-li-x</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>te-szub-na-sir</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>ip-qu2-isz8-tar2</t>
-        </is>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>P509669.conll</t>
+          <t>P122478.conll</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>gu4-ab2</t>
+          <t>ur-{d}ku3-SZIM</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>amar-ga</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>la-lum</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>x-x-x-x</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>gu4-ab2</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>amar-ga</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>la-lum</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>x-x-x-x</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>la-lu-um</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>sa-al-lum</t>
+          <t>da-da-mu-ta</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>P509670.conll</t>
+          <t>P122479.conll</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -827,112 +657,527 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>gu4-ab2</t>
+          <t>lu2-sa6-ga</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>amar-ga</t>
+          <t>ur-ma-ma</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>amar-ga</t>
+          <t>dingir-gu2-sa6</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>gu4-ab2</t>
+          <t>ur-{d}suen</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>amar-ga</t>
+          <t>lu2-...</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>amar-ga</t>
+          <t>ur-{d}...</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>P509671.conll</t>
+          <t>P122480.conll</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>amar-ga</t>
+          <t>lu2-{d}ba-ba6</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>amar-ga</t>
+          <t>lu2-{d}nanna</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>dingir-na-sir</t>
+          <t>...</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>amar-ga</t>
+          <t>...</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>amar-ga</t>
+          <t>...</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>er3-ra-ha-bi-it</t>
+          <t>...</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>amar-ga</t>
+          <t>...</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>amar-ga</t>
+          <t>...-tum</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>amar-ga</t>
+          <t>ur-me-me</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>amar-ga</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>amar-ga</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>a-hu-um-ma</t>
-        </is>
-      </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>amar-ga</t>
-        </is>
-      </c>
-      <c r="P10" t="inlineStr">
-        <is>
-          <t>{d}suen-na-si-ir</t>
+          <t>...</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>P122481.conll</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>3</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>i-di3-{d}iszkur</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>lugal-ma2-gur8-re</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>a2-ba</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>P122482.conll</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>eb2-gul</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>P122483.conll</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>4</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>ur-{d}en-lil2-la2-ke4</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>ma2-gur8-mah</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>ur-{d}en-lil2-la2</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>lugal-he2-gal2</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>P122484.conll</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>3</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>lu2-...</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>lu2-{d}inanna</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>lu2-x-x</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>P312786.conll</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>7</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>lu2-dingir-ra</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>he2-ma-du</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>gu-u2-gu-a</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>tu-ra</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>u2-li</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>gu-u2-gu-a</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>ma-an-szum2</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>P312789.conll</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>5</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>ur-{d}en-lil2-la2</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>ur-{gesz}gigir</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>szesz-kal-la</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>lugal-nig2-lagar-e</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>da-da</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>P312790.conll</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>6</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>szesz-saga</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>da-da-ga</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>lugal-ku3-zu</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>en-unu6-gal</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>lugal-ku3-zu</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>ur-nigar{gar}</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>P312791.conll</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>3</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>du10-ga-mu</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>du10-ga-mu</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>a-asz-an-ne2</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>P312792.conll</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>4</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>e2-duru5-NE-sze3</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>a-kal-la</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>a-kal-la</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>ur-nigar{gar}</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>P312793.conll</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>3</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>szu-palil2</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>ka-ku3</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>lugal-i3-sa6-ga</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>P312794.conll</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>5</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>...</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>asz-a</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>geme2-{d}a-szar2</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>ma2-gur8-mah</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>geme2-{d}a-szar2</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>P313083.conll</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>4</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>ur-{d}ba-ba6</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>en-unu6-gal</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>lu2-kal-la</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>ur-nigar{gar}</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>P313084.conll</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>P313085.conll</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>6</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>lugal-amar-ku3</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>ur-nigar{gar}</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>lugal-nesag-e</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>lugal-nesag-e</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>en-unu6-gal</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>lugal-nesag-e</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>P313086.conll</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>3</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>ur-x-sukkal</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>ur-sukkal</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>ur-x</t>
         </is>
       </c>
     </row>
@@ -947,10 +1192,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R11"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
@@ -970,224 +1215,344 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>P509633.conll</t>
+          <t>P122472.conll</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">mu {d}nin-urta u3 ma-na-ba-al-te-el in-pa3 igi ia-ah-zi-be2-el3 dumu isz-me-{d}suen igi szu-la-ra-ak igi na-nu-szu-um dumu za-x-la-nu igi ku-nu-um dumu nu-ur2-ia </t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">mu e2 {d}nin-urta ma-na-ba-al-te-el mu-na-du3 dumu isz-me-{d}suen igi szu-la-ra-ak dumu x-x-x-x igi ku-nu-um dumu nu-ur2-ia ... x ... </t>
-        </is>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>P509634.conll</t>
+          <t>P122473.conll</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mu ma2-gur8-mah ba-ab-du8 </t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>P509636.conll</t>
+          <t>P122474.conll</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">mu {gesz}gu-za za3-bi-us2 3(disz)-a-bi {d}en-lil2 {d}nin-urta {d}nin-nibru{ki} ma-na-ba-al-te-el {disz}{d}suen-a-hu-szu u3 sza-at-{d}gibil6 ha-la e2 ad-da-ni nig2 na-me ugu za-za-kum li-bi2-in-tuku igi a-mur-i-lu-su2 igi {d}suen-en-nam szitim igi bur-ia dumu sa-li igi {d}nanna-zi-sza3-gal2 iti gan-gan-e3 </t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">mu {gesz}gu-za za3-bi-us2 3(disz)-a-bi {d}en-lil2 {d}nin-urta {d}nin-nibru{ki} ma-na-dim2 {d}suen-a-bu-szu dumu za-pa-ti </t>
-        </is>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>P509663.conll</t>
+          <t>P122475.conll</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t xml:space="preserve">mu ma-ma-ba-al-te-el 6(disz) gin2 ku3-babbar sa10 2(asz) gur sze szu ti-a a-na-gum </t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">mu mu-na-ba-al-te-el 1(u) 3(disz) 1/2(disz) gin2 1(disz)-kam 1(u) 3(disz) 1/3(disz) gin2 2(disz)-kam 1/3(disz) ma-na 8(disz) igi-6(disz)-gal2 szu-la2 </t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">mu ma-na-ba-al-te-el </t>
+          <t xml:space="preserve">mu en masz2-e ib2-pa3 </t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>P509664.conll</t>
+          <t>P122476.conll</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mu lugal-bi i3-pa3 </t>
+        </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>P509668.conll</t>
+          <t>P122477.conll</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mu ma-da za-ab-sza-li{ki} ba-hul </t>
+        </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>P509669.conll</t>
+          <t>P122478.conll</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t xml:space="preserve">mu ... 4(disz) gu4-ab2 6(disz) ab2 mah2 2(u) 7(disz) gu4 amar-ga 1(disz) amar nig2 e2 nam-ra-tum nig2-szu la-lum giri3 x-x-x-x i3-gen-ne-en iti sze-sag11-ku5 u4 4(disz)-kam </t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">mu GISZ ... la-lu-um dumu sa-al-lum </t>
+          <t xml:space="preserve">mu e2 {d}szara2 umma{ki} ba-du3 </t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>P509670.conll</t>
+          <t>P122479.conll</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">mu ... 4(disz) ab2 mah2 6(disz) gu4-ab2 2(u) 2(disz) ab2 amar-ga 6(disz) gu4 amar-ga 3(u) 8(disz) gu4 ab2 amar-hi-a nig2-szu {d}utu-sipa </t>
-        </is>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>P509671.conll</t>
+          <t>P122480.conll</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>16</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">mu 1(disz) 2(disz) gu4 </t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">mu 2(disz) 1(disz) gu4 </t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">mu 1(disz) 1(disz) gu4 amar-ga 1(disz) ab2 amar-ga 1(u) 1(disz) gu4 ab2 amar dingir-na-sir 2(disz) ab2 mah2 2(disz) ab2 </t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">mu 1(disz) 1(disz) ab2 amar-ga 1(disz) gu4 amar-ga 6(disz) er3-ra-ha-bi-it 4(disz) ab2 mah2 2(disz) ab2 amar-ga 1(disz) gu4 amar-ga n ab2 amar-ga n ab2 </t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">mu n n gu4 </t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">mu 2(disz) 1(disz) gu4 </t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">mu 1(disz) 1(disz) gu4 amar-ga 1(disz) ab2 amar-ga 8(disz) a-hu-um-ma 1(disz) ab2 mah2 1(disz) gu4 </t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">mu 3(disz) 1(disz) gu4 </t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">mu 1(disz) 1(disz) ab2 amar-ga 4(disz) {d}suen-na-si-ir 2(disz) ab2 mah2 2(disz) ab2 </t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">mu 2(disz) 1(disz) gu4 </t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">mu n 5(disz) sza3 2(u) a-ra2 1(disz)-kam 5(disz) ab2 mah2 2(disz) ab2 </t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">mu 2(disz) 2(disz) ab2 </t>
-        </is>
-      </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">mu 1(disz) 2(disz) gu4 </t>
-        </is>
-      </c>
-      <c r="P10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">mu 1(disz) 3(disz) gu4 </t>
-        </is>
-      </c>
-      <c r="Q10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">mu 2(disz) 3(disz) gu4 </t>
-        </is>
-      </c>
-      <c r="R10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">mu 3(disz) 1(u) 7(disz) x ... nig2-szu {d}suen-x-x </t>
-        </is>
-      </c>
-    </row>
-    <row r="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>P122481.conll</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>P122482.conll</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mu si-ma-num2{ki} ba-hul-a </t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>P122483.conll</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mu ma2-gur8-mah ba-dim2 </t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>P122484.conll</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mu ma2-dara4-abzu ba-ab-du8 </t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>P312786.conll</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>2</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mu na-ru2-a-mah ba-du3-ta </t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mu ma-da za-ab-sza-li{ki} ba-hul </t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>P312789.conll</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mu gu-za {d}en-lil2-la2 ba-dim2 </t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>P312790.conll</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mu us2-sa </t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>P312791.conll</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mu ha-ar-szi{ki} ba-hul </t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>P312792.conll</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mu us2-sa </t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>P312793.conll</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mu us2-sa </t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>P312794.conll</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mu {d}szu-{d}suen lugal-e ma2-gur8-mah {d}en-lil2 {d}nin-lil2-ra ba-dim2 </t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>P313083.conll</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>1</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mu en-unu6-gal {d}inanna ba-hun </t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>P313084.conll</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>1</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mu ki-masz{ki} ba-hul </t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>P313085.conll</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>1</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mu en-unu6-gal {d}inanna ba-hun </t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>P313086.conll</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>1</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mu ur-bi2-i3-lum{ki} ba-hul </t>
+        </is>
+      </c>
+    </row>
+    <row r="26"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1199,10 +1564,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
@@ -1227,136 +1592,361 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>P509633.conll</t>
+          <t>P122472.conll</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>sulgi 42a</t>
+          <t>start</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.3173076923076923</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>P509634.conll</t>
+          <t>P122473.conll</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>start</t>
+          <t>sulgi 8</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>0.7213114754098361</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>P509636.conll</t>
+          <t>P122474.conll</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>sulgi 3</t>
+          <t>start</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.387434554973822</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>P509663.conll</t>
+          <t>P122475.conll</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ur-namma 9</t>
+          <t>ur-namma 8</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.5714285714285714</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>P509664.conll</t>
+          <t>P122476.conll</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>start</t>
+          <t>su-suen 1b</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>0.5365853658536586</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>P509668.conll</t>
+          <t>P122477.conll</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>start</t>
+          <t>su-suen 8a</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>0.7826086956521739</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>P509669.conll</t>
+          <t>P122478.conll</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>sulgi 48a</t>
+          <t>ur-namma 7</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.4210526315789473</v>
+        <v>0.5660377358490566</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>P509670.conll</t>
+          <t>P122479.conll</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>sulgi 27a</t>
+          <t>start</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.2761506276150628</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>P509671.conll</t>
+          <t>P122480.conll</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ur-namma 9</t>
+          <t>start</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.4375</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>P122481.conll</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>start</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>P122482.conll</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>sulgi 25b</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>P122483.conll</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>sulgi 8</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>0.576271186440678</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>P122484.conll</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>su-suen 3a</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>0.6493506493506493</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>P312786.conll</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>su-suen 8a</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>0.7826086956521739</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>P312789.conll</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>sulgi 16</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>0.6666666666666666</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>P312790.conll</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>su-suen 2a</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>0.5714285714285714</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>P312791.conll</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>sulgi 27b</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>0.8636363636363636</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>P312792.conll</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>su-suen 2a</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>0.5714285714285714</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>P312793.conll</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>su-suen 2a</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>0.5714285714285714</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>P312794.conll</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>su-suen 8b</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>0.7152317880794702</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>P313083.conll</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>ibbi-suen 4b</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>0.7352941176470589</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>P313084.conll</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>sulgi 47a</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>0.723404255319149</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>P313085.conll</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>ibbi-suen 4b</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>0.7352941176470589</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>P313086.conll</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>sulgi 46a</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>0.7368421052631579</v>
       </c>
     </row>
   </sheetData>

</xml_diff>